<commit_message>
moved testing to Mac
</commit_message>
<xml_diff>
--- a/client/test_results/filtered_chrome_test_results.xlsx
+++ b/client/test_results/filtered_chrome_test_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.383191823959351</v>
+        <v>0.7616477012634277</v>
       </c>
       <c r="D2" t="n">
         <v>7.972</v>
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.02782940864563</v>
+        <v>0.452197790145874</v>
       </c>
       <c r="D3" t="n">
         <v>7.972</v>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9148445129394531</v>
+        <v>0.5917079448699951</v>
       </c>
       <c r="D4" t="n">
         <v>7.308</v>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7391419410705566</v>
+        <v>0.6104588508605957</v>
       </c>
       <c r="D5" t="n">
         <v>7.308</v>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3374981880187988</v>
+        <v>0.2285418510437012</v>
       </c>
       <c r="D6" t="n">
         <v>6.017</v>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4890260696411133</v>
+        <v>0.218609094619751</v>
       </c>
       <c r="D7" t="n">
         <v>6.017</v>
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3514533042907715</v>
+        <v>0.2316949367523193</v>
       </c>
       <c r="D8" t="n">
         <v>5.353</v>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3610293865203857</v>
+        <v>0.2334060668945312</v>
       </c>
       <c r="D9" t="n">
         <v>5.353</v>
@@ -593,7 +593,7 @@
         <v>100</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4713866710662842</v>
+        <v>0.3044748306274414</v>
       </c>
       <c r="D10" t="n">
         <v>67.27800000000001</v>
@@ -609,7 +609,7 @@
         <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4817965030670166</v>
+        <v>0.2564606666564941</v>
       </c>
       <c r="D11" t="n">
         <v>73.413</v>
@@ -625,7 +625,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="n">
-        <v>7.96736478805542</v>
+        <v>1.385181188583374</v>
       </c>
       <c r="D12" t="n">
         <v>56.173</v>
@@ -641,7 +641,7 @@
         <v>100</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9489290714263916</v>
+        <v>0.7043569087982178</v>
       </c>
       <c r="D13" t="n">
         <v>73.245</v>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7504003047943115</v>
+        <v>0.46120285987854</v>
       </c>
       <c r="D14" t="n">
         <v>8.17</v>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7461929321289062</v>
+        <v>0.4641599655151367</v>
       </c>
       <c r="D15" t="n">
         <v>8.17</v>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8938493728637695</v>
+        <v>0.6073551177978516</v>
       </c>
       <c r="D16" t="n">
         <v>7.326</v>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.093066453933716</v>
+        <v>0.6166253089904785</v>
       </c>
       <c r="D17" t="n">
         <v>7.326</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5906622409820557</v>
+        <v>0.2390539646148682</v>
       </c>
       <c r="D18" t="n">
         <v>6.215</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4378812313079834</v>
+        <v>0.2097170352935791</v>
       </c>
       <c r="D19" t="n">
         <v>6.215</v>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5148677825927734</v>
+        <v>0.2335460186004639</v>
       </c>
       <c r="D20" t="n">
         <v>5.371</v>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5227210521697998</v>
+        <v>0.2475011348724365</v>
       </c>
       <c r="D21" t="n">
         <v>5.371</v>
@@ -785,7 +785,7 @@
         <v>100</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5470459461212158</v>
+        <v>0.2984390258789062</v>
       </c>
       <c r="D22" t="n">
         <v>64.398</v>
@@ -801,7 +801,7 @@
         <v>100</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5539813041687012</v>
+        <v>0.2853021621704102</v>
       </c>
       <c r="D23" t="n">
         <v>522.806</v>
@@ -817,7 +817,7 @@
         <v>100</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9528276920318604</v>
+        <v>0.7291519641876221</v>
       </c>
       <c r="D24" t="n">
         <v>58.093</v>
@@ -833,7 +833,7 @@
         <v>100</v>
       </c>
       <c r="C25" t="n">
-        <v>1.17426872253418</v>
+        <v>0.8237051963806152</v>
       </c>
       <c r="D25" t="n">
         <v>522.668</v>

</xml_diff>

<commit_message>
encryption experiment ready for testing
</commit_message>
<xml_diff>
--- a/client/test_results/filtered_chrome_test_results.xlsx
+++ b/client/test_results/filtered_chrome_test_results.xlsx
@@ -465,10 +465,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.866541862487793</v>
+        <v>2.255192041397095</v>
       </c>
       <c r="D2" t="n">
-        <v>113.882</v>
+        <v>115.378</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8198010921478271</v>
+        <v>0.06632399559020996</v>
       </c>
       <c r="D3" t="n">
-        <v>113.882</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -497,10 +497,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7825679779052734</v>
+        <v>0.06693005561828613</v>
       </c>
       <c r="D4" t="n">
-        <v>36.058</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -513,10 +513,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7832520008087158</v>
+        <v>0.07197117805480957</v>
       </c>
       <c r="D5" t="n">
-        <v>36.058</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>0.442882776260376</v>
+        <v>0.06642889976501465</v>
       </c>
       <c r="D6" t="n">
-        <v>34.767</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4710469245910645</v>
+        <v>0.06895995140075684</v>
       </c>
       <c r="D7" t="n">
-        <v>34.767</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -561,10 +561,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4457030296325684</v>
+        <v>0.06762409210205078</v>
       </c>
       <c r="D8" t="n">
-        <v>34.103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -577,10 +577,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4514479637145996</v>
+        <v>0.06976199150085449</v>
       </c>
       <c r="D9" t="n">
-        <v>34.103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -593,10 +593,10 @@
         <v>100</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4471509456634521</v>
+        <v>0.06574010848999023</v>
       </c>
       <c r="D10" t="n">
-        <v>96.02800000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -609,10 +609,10 @@
         <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4793989658355713</v>
+        <v>0.06995487213134766</v>
       </c>
       <c r="D11" t="n">
-        <v>102.163</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.702942132949829</v>
+        <v>0.06684327125549316</v>
       </c>
       <c r="D12" t="n">
-        <v>162.083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">

</xml_diff>